<commit_message>
Testing new step2 on scanner dataset ok
</commit_message>
<xml_diff>
--- a/raw/project_Other_standardizer.xlsx
+++ b/raw/project_Other_standardizer.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18380" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18380" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Metadata" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,12 +49,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -84,13 +99,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3035,7 +3050,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>sample_cruise_haul_net_id</t>
+          <t>sample_id</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -7453,7 +7468,7 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testing scripts 0-2 with new Zooscan projects ok.
</commit_message>
<xml_diff>
--- a/raw/project_Other_standardizer.xlsx
+++ b/raw/project_Other_standardizer.xlsx
@@ -7468,24 +7468,24 @@
   </sheetPr>
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Variables</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Variable_types</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Description</t>
         </is>

</xml_diff>